<commit_message>
Updated results of missing sd pair (stackoverflow_formatted/19051537_0.java)
- It is an error fragment
</commit_message>
<xml_diff>
--- a/results/missing_sdf_pairs.xlsx
+++ b/results/missing_sdf_pairs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -291,10 +291,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -320,11 +327,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,7 +616,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,7 +628,7 @@
     <col min="5" max="5" width="36.5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="57.5" customWidth="1"/>
+    <col min="9" max="9" width="133.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2" hidden="1" customWidth="1"/>
@@ -1974,59 +1985,59 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" t="s">
+    <row r="26" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>2</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>65</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
         <v>64</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="3">
         <v>34</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="3">
         <v>97</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="3">
         <v>64</v>
       </c>
-      <c r="M26" t="s">
-        <v>1</v>
-      </c>
-      <c r="N26" t="s">
+      <c r="M26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="O26" s="3">
+        <v>1</v>
+      </c>
+      <c r="P26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="Q26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R26" s="1" t="s">
+      <c r="R26" s="2" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>